<commit_message>
resolve gh issue #17, band-aid solution to issue #26
</commit_message>
<xml_diff>
--- a/Code/Photologic Rig Main Application Code/data_outputs/Experiment Schedule, 2025-03-17.xlsx
+++ b/Code/Photologic Rig Main Application Code/data_outputs/Experiment Schedule, 2025-03-17.xlsx
@@ -506,7 +506,7 @@
         <v>0</v>
       </c>
       <c r="F2" t="n">
-        <v>0</v>
+        <v>159</v>
       </c>
       <c r="G2" t="n">
         <v>5000</v>
@@ -518,7 +518,7 @@
         <v>5000</v>
       </c>
       <c r="J2" t="n">
-        <v>5000</v>
+        <v>54.50153350830078</v>
       </c>
     </row>
     <row r="3">
@@ -539,10 +539,10 @@
         </is>
       </c>
       <c r="E3" t="n">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="F3" t="n">
-        <v>28</v>
+        <v>159</v>
       </c>
       <c r="G3" t="n">
         <v>5000</v>
@@ -554,7 +554,7 @@
         <v>5000</v>
       </c>
       <c r="J3" t="n">
-        <v>738.72971534729</v>
+        <v>186.4371299743652</v>
       </c>
     </row>
     <row r="4">
@@ -566,19 +566,19 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
+          <t>sac</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
           <t>suc</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>sac</t>
-        </is>
-      </c>
       <c r="E4" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="F4" t="n">
-        <v>25</v>
+        <v>160</v>
       </c>
       <c r="G4" t="n">
         <v>5000</v>
@@ -590,7 +590,7 @@
         <v>5000</v>
       </c>
       <c r="J4" t="n">
-        <v>897.7396488189697</v>
+        <v>191.0860538482666</v>
       </c>
     </row>
     <row r="5">
@@ -602,19 +602,19 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
+          <t>suc</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
           <t>sac</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>suc</t>
         </is>
       </c>
       <c r="E5" t="n">
         <v>0</v>
       </c>
       <c r="F5" t="n">
-        <v>32</v>
+        <v>160</v>
       </c>
       <c r="G5" t="n">
         <v>5000</v>
@@ -626,7 +626,7 @@
         <v>5000</v>
       </c>
       <c r="J5" t="n">
-        <v>1651.840925216675</v>
+        <v>193.4034824371338</v>
       </c>
     </row>
     <row r="6">
@@ -650,7 +650,7 @@
         <v>0</v>
       </c>
       <c r="F6" t="n">
-        <v>30</v>
+        <v>160</v>
       </c>
       <c r="G6" t="n">
         <v>5000</v>
@@ -662,7 +662,7 @@
         <v>5000</v>
       </c>
       <c r="J6" t="n">
-        <v>651.0593891143799</v>
+        <v>193.6280727386475</v>
       </c>
     </row>
     <row r="7">
@@ -683,10 +683,10 @@
         </is>
       </c>
       <c r="E7" t="n">
-        <v>27</v>
+        <v>0</v>
       </c>
       <c r="F7" t="n">
-        <v>0</v>
+        <v>160</v>
       </c>
       <c r="G7" t="n">
         <v>5000</v>
@@ -698,7 +698,7 @@
         <v>5000</v>
       </c>
       <c r="J7" t="n">
-        <v>652.4214744567871</v>
+        <v>196.1033344268799</v>
       </c>
     </row>
     <row r="8">
@@ -722,7 +722,7 @@
         <v>0</v>
       </c>
       <c r="F8" t="n">
-        <v>0</v>
+        <v>160</v>
       </c>
       <c r="G8" t="n">
         <v>5000</v>
@@ -734,7 +734,7 @@
         <v>5000</v>
       </c>
       <c r="J8" t="n">
-        <v>5000</v>
+        <v>195.2712535858154</v>
       </c>
     </row>
     <row r="9">
@@ -758,7 +758,7 @@
         <v>0</v>
       </c>
       <c r="F9" t="n">
-        <v>0</v>
+        <v>160</v>
       </c>
       <c r="G9" t="n">
         <v>5000</v>
@@ -769,7 +769,9 @@
       <c r="I9" t="n">
         <v>5000</v>
       </c>
-      <c r="J9" t="inlineStr"/>
+      <c r="J9" t="n">
+        <v>193.2954788208008</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
fix issues #20, #26
</commit_message>
<xml_diff>
--- a/Code/Photologic Rig Main Application Code/data_outputs/Experiment Schedule, 2025-03-17.xlsx
+++ b/Code/Photologic Rig Main Application Code/data_outputs/Experiment Schedule, 2025-03-17.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J9"/>
+  <dimension ref="A1:J41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -494,19 +494,19 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>suc</t>
+          <t>sour</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>sac</t>
+          <t>sweet</t>
         </is>
       </c>
       <c r="E2" t="n">
-        <v>0</v>
+        <v>65</v>
       </c>
       <c r="F2" t="n">
-        <v>159</v>
+        <v>41</v>
       </c>
       <c r="G2" t="n">
         <v>5000</v>
@@ -518,7 +518,7 @@
         <v>5000</v>
       </c>
       <c r="J2" t="n">
-        <v>54.50153350830078</v>
+        <v>104.0654182434082</v>
       </c>
     </row>
     <row r="3">
@@ -530,19 +530,19 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>sac</t>
+          <t>sucrose</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>suc</t>
+          <t>saccarhin</t>
         </is>
       </c>
       <c r="E3" t="n">
         <v>0</v>
       </c>
       <c r="F3" t="n">
-        <v>159</v>
+        <v>106</v>
       </c>
       <c r="G3" t="n">
         <v>5000</v>
@@ -554,31 +554,31 @@
         <v>5000</v>
       </c>
       <c r="J3" t="n">
-        <v>186.4371299743652</v>
+        <v>162.2185707092285</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B4" t="n">
         <v>3</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>sac</t>
+          <t>saccarhin</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>suc</t>
+          <t>sucrose</t>
         </is>
       </c>
       <c r="E4" t="n">
         <v>0</v>
       </c>
       <c r="F4" t="n">
-        <v>160</v>
+        <v>106</v>
       </c>
       <c r="G4" t="n">
         <v>5000</v>
@@ -590,31 +590,31 @@
         <v>5000</v>
       </c>
       <c r="J4" t="n">
-        <v>191.0860538482666</v>
+        <v>169.8324680328369</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B5" t="n">
         <v>4</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>suc</t>
+          <t>sweet</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>sac</t>
+          <t>sour</t>
         </is>
       </c>
       <c r="E5" t="n">
         <v>0</v>
       </c>
       <c r="F5" t="n">
-        <v>160</v>
+        <v>106</v>
       </c>
       <c r="G5" t="n">
         <v>5000</v>
@@ -626,31 +626,31 @@
         <v>5000</v>
       </c>
       <c r="J5" t="n">
-        <v>193.4034824371338</v>
+        <v>174.0574836730957</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B6" t="n">
         <v>5</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>suc</t>
+          <t>sweet</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>sac</t>
+          <t>sour</t>
         </is>
       </c>
       <c r="E6" t="n">
-        <v>0</v>
+        <v>107</v>
       </c>
       <c r="F6" t="n">
-        <v>160</v>
+        <v>0</v>
       </c>
       <c r="G6" t="n">
         <v>5000</v>
@@ -662,31 +662,31 @@
         <v>5000</v>
       </c>
       <c r="J6" t="n">
-        <v>193.6280727386475</v>
+        <v>171.3287830352783</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B7" t="n">
         <v>6</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>sac</t>
+          <t>saccarhin</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>suc</t>
+          <t>sucrose</t>
         </is>
       </c>
       <c r="E7" t="n">
-        <v>0</v>
+        <v>106</v>
       </c>
       <c r="F7" t="n">
-        <v>160</v>
+        <v>0</v>
       </c>
       <c r="G7" t="n">
         <v>5000</v>
@@ -698,31 +698,31 @@
         <v>5000</v>
       </c>
       <c r="J7" t="n">
-        <v>196.1033344268799</v>
+        <v>177.3412227630615</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B8" t="n">
         <v>7</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>sac</t>
+          <t>sour</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>suc</t>
+          <t>sweet</t>
         </is>
       </c>
       <c r="E8" t="n">
-        <v>0</v>
+        <v>106</v>
       </c>
       <c r="F8" t="n">
-        <v>160</v>
+        <v>0</v>
       </c>
       <c r="G8" t="n">
         <v>5000</v>
@@ -734,31 +734,31 @@
         <v>5000</v>
       </c>
       <c r="J8" t="n">
-        <v>195.2712535858154</v>
+        <v>174.0810871124268</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B9" t="n">
         <v>8</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>suc</t>
+          <t>sucrose</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>sac</t>
+          <t>saccarhin</t>
         </is>
       </c>
       <c r="E9" t="n">
-        <v>0</v>
+        <v>106</v>
       </c>
       <c r="F9" t="n">
-        <v>160</v>
+        <v>0</v>
       </c>
       <c r="G9" t="n">
         <v>5000</v>
@@ -770,7 +770,1159 @@
         <v>5000</v>
       </c>
       <c r="J9" t="n">
-        <v>193.2954788208008</v>
+        <v>174.0903854370117</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>3</v>
+      </c>
+      <c r="B10" t="n">
+        <v>9</v>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>sour</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>sweet</t>
+        </is>
+      </c>
+      <c r="E10" t="n">
+        <v>0</v>
+      </c>
+      <c r="F10" t="n">
+        <v>107</v>
+      </c>
+      <c r="G10" t="n">
+        <v>5000</v>
+      </c>
+      <c r="H10" t="n">
+        <v>5000</v>
+      </c>
+      <c r="I10" t="n">
+        <v>5000</v>
+      </c>
+      <c r="J10" t="n">
+        <v>175.2786636352539</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>3</v>
+      </c>
+      <c r="B11" t="n">
+        <v>10</v>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>sweet</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>sour</t>
+        </is>
+      </c>
+      <c r="E11" t="n">
+        <v>0</v>
+      </c>
+      <c r="F11" t="n">
+        <v>106</v>
+      </c>
+      <c r="G11" t="n">
+        <v>5000</v>
+      </c>
+      <c r="H11" t="n">
+        <v>5000</v>
+      </c>
+      <c r="I11" t="n">
+        <v>5000</v>
+      </c>
+      <c r="J11" t="n">
+        <v>176.1007308959961</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>3</v>
+      </c>
+      <c r="B12" t="n">
+        <v>11</v>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>saccarhin</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>sucrose</t>
+        </is>
+      </c>
+      <c r="E12" t="n">
+        <v>0</v>
+      </c>
+      <c r="F12" t="n">
+        <v>106</v>
+      </c>
+      <c r="G12" t="n">
+        <v>5000</v>
+      </c>
+      <c r="H12" t="n">
+        <v>5000</v>
+      </c>
+      <c r="I12" t="n">
+        <v>5000</v>
+      </c>
+      <c r="J12" t="n">
+        <v>177.9711246490479</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>3</v>
+      </c>
+      <c r="B13" t="n">
+        <v>12</v>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>sucrose</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>saccarhin</t>
+        </is>
+      </c>
+      <c r="E13" t="n">
+        <v>101</v>
+      </c>
+      <c r="F13" t="n">
+        <v>5</v>
+      </c>
+      <c r="G13" t="n">
+        <v>5000</v>
+      </c>
+      <c r="H13" t="n">
+        <v>5000</v>
+      </c>
+      <c r="I13" t="n">
+        <v>5000</v>
+      </c>
+      <c r="J13" t="n">
+        <v>174.6385097503662</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>4</v>
+      </c>
+      <c r="B14" t="n">
+        <v>13</v>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>sucrose</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>saccarhin</t>
+        </is>
+      </c>
+      <c r="E14" t="n">
+        <v>106</v>
+      </c>
+      <c r="F14" t="n">
+        <v>0</v>
+      </c>
+      <c r="G14" t="n">
+        <v>5000</v>
+      </c>
+      <c r="H14" t="n">
+        <v>5000</v>
+      </c>
+      <c r="I14" t="n">
+        <v>5000</v>
+      </c>
+      <c r="J14" t="n">
+        <v>179.9426078796387</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>4</v>
+      </c>
+      <c r="B15" t="n">
+        <v>14</v>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>sour</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>sweet</t>
+        </is>
+      </c>
+      <c r="E15" t="n">
+        <v>106</v>
+      </c>
+      <c r="F15" t="n">
+        <v>0</v>
+      </c>
+      <c r="G15" t="n">
+        <v>5000</v>
+      </c>
+      <c r="H15" t="n">
+        <v>5000</v>
+      </c>
+      <c r="I15" t="n">
+        <v>5000</v>
+      </c>
+      <c r="J15" t="n">
+        <v>174.2255687713623</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>4</v>
+      </c>
+      <c r="B16" t="n">
+        <v>15</v>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>sweet</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>sour</t>
+        </is>
+      </c>
+      <c r="E16" t="n">
+        <v>106</v>
+      </c>
+      <c r="F16" t="n">
+        <v>0</v>
+      </c>
+      <c r="G16" t="n">
+        <v>5000</v>
+      </c>
+      <c r="H16" t="n">
+        <v>5000</v>
+      </c>
+      <c r="I16" t="n">
+        <v>5000</v>
+      </c>
+      <c r="J16" t="n">
+        <v>176.1066913604736</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>4</v>
+      </c>
+      <c r="B17" t="n">
+        <v>16</v>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>saccarhin</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>sucrose</t>
+        </is>
+      </c>
+      <c r="E17" t="n">
+        <v>0</v>
+      </c>
+      <c r="F17" t="n">
+        <v>106</v>
+      </c>
+      <c r="G17" t="n">
+        <v>5000</v>
+      </c>
+      <c r="H17" t="n">
+        <v>5000</v>
+      </c>
+      <c r="I17" t="n">
+        <v>5000</v>
+      </c>
+      <c r="J17" t="n">
+        <v>173.9847660064697</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>5</v>
+      </c>
+      <c r="B18" t="n">
+        <v>17</v>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>sweet</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>sour</t>
+        </is>
+      </c>
+      <c r="E18" t="n">
+        <v>0</v>
+      </c>
+      <c r="F18" t="n">
+        <v>106</v>
+      </c>
+      <c r="G18" t="n">
+        <v>5000</v>
+      </c>
+      <c r="H18" t="n">
+        <v>5000</v>
+      </c>
+      <c r="I18" t="n">
+        <v>5000</v>
+      </c>
+      <c r="J18" t="n">
+        <v>177.2794723510742</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>5</v>
+      </c>
+      <c r="B19" t="n">
+        <v>18</v>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>sucrose</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>saccarhin</t>
+        </is>
+      </c>
+      <c r="E19" t="n">
+        <v>0</v>
+      </c>
+      <c r="F19" t="n">
+        <v>106</v>
+      </c>
+      <c r="G19" t="n">
+        <v>5000</v>
+      </c>
+      <c r="H19" t="n">
+        <v>5000</v>
+      </c>
+      <c r="I19" t="n">
+        <v>5000</v>
+      </c>
+      <c r="J19" t="n">
+        <v>175.8193969726562</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>5</v>
+      </c>
+      <c r="B20" t="n">
+        <v>19</v>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>saccarhin</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>sucrose</t>
+        </is>
+      </c>
+      <c r="E20" t="n">
+        <v>49</v>
+      </c>
+      <c r="F20" t="n">
+        <v>57</v>
+      </c>
+      <c r="G20" t="n">
+        <v>5000</v>
+      </c>
+      <c r="H20" t="n">
+        <v>5000</v>
+      </c>
+      <c r="I20" t="n">
+        <v>5000</v>
+      </c>
+      <c r="J20" t="n">
+        <v>176.1937141418457</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>5</v>
+      </c>
+      <c r="B21" t="n">
+        <v>20</v>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>sour</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>sweet</t>
+        </is>
+      </c>
+      <c r="E21" t="n">
+        <v>106</v>
+      </c>
+      <c r="F21" t="n">
+        <v>0</v>
+      </c>
+      <c r="G21" t="n">
+        <v>5000</v>
+      </c>
+      <c r="H21" t="n">
+        <v>5000</v>
+      </c>
+      <c r="I21" t="n">
+        <v>5000</v>
+      </c>
+      <c r="J21" t="n">
+        <v>178.0130863189697</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>6</v>
+      </c>
+      <c r="B22" t="n">
+        <v>21</v>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>sour</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>sweet</t>
+        </is>
+      </c>
+      <c r="E22" t="n">
+        <v>106</v>
+      </c>
+      <c r="F22" t="n">
+        <v>0</v>
+      </c>
+      <c r="G22" t="n">
+        <v>5000</v>
+      </c>
+      <c r="H22" t="n">
+        <v>5000</v>
+      </c>
+      <c r="I22" t="n">
+        <v>5000</v>
+      </c>
+      <c r="J22" t="n">
+        <v>175.8208274841309</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>6</v>
+      </c>
+      <c r="B23" t="n">
+        <v>22</v>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>sucrose</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>saccarhin</t>
+        </is>
+      </c>
+      <c r="E23" t="n">
+        <v>106</v>
+      </c>
+      <c r="F23" t="n">
+        <v>0</v>
+      </c>
+      <c r="G23" t="n">
+        <v>5000</v>
+      </c>
+      <c r="H23" t="n">
+        <v>5000</v>
+      </c>
+      <c r="I23" t="n">
+        <v>5000</v>
+      </c>
+      <c r="J23" t="n">
+        <v>174.8189926147461</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>6</v>
+      </c>
+      <c r="B24" t="n">
+        <v>23</v>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>sweet</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>sour</t>
+        </is>
+      </c>
+      <c r="E24" t="n">
+        <v>0</v>
+      </c>
+      <c r="F24" t="n">
+        <v>106</v>
+      </c>
+      <c r="G24" t="n">
+        <v>5000</v>
+      </c>
+      <c r="H24" t="n">
+        <v>5000</v>
+      </c>
+      <c r="I24" t="n">
+        <v>5000</v>
+      </c>
+      <c r="J24" t="n">
+        <v>175.2340793609619</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>6</v>
+      </c>
+      <c r="B25" t="n">
+        <v>24</v>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>saccarhin</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>sucrose</t>
+        </is>
+      </c>
+      <c r="E25" t="n">
+        <v>0</v>
+      </c>
+      <c r="F25" t="n">
+        <v>106</v>
+      </c>
+      <c r="G25" t="n">
+        <v>5000</v>
+      </c>
+      <c r="H25" t="n">
+        <v>5000</v>
+      </c>
+      <c r="I25" t="n">
+        <v>5000</v>
+      </c>
+      <c r="J25" t="n">
+        <v>175.2972602844238</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>7</v>
+      </c>
+      <c r="B26" t="n">
+        <v>25</v>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>sucrose</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>saccarhin</t>
+        </is>
+      </c>
+      <c r="E26" t="n">
+        <v>0</v>
+      </c>
+      <c r="F26" t="n">
+        <v>106</v>
+      </c>
+      <c r="G26" t="n">
+        <v>5000</v>
+      </c>
+      <c r="H26" t="n">
+        <v>5000</v>
+      </c>
+      <c r="I26" t="n">
+        <v>5000</v>
+      </c>
+      <c r="J26" t="n">
+        <v>176.5103340148926</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>7</v>
+      </c>
+      <c r="B27" t="n">
+        <v>26</v>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>saccarhin</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>sucrose</t>
+        </is>
+      </c>
+      <c r="E27" t="n">
+        <v>0</v>
+      </c>
+      <c r="F27" t="n">
+        <v>107</v>
+      </c>
+      <c r="G27" t="n">
+        <v>5000</v>
+      </c>
+      <c r="H27" t="n">
+        <v>5000</v>
+      </c>
+      <c r="I27" t="n">
+        <v>5000</v>
+      </c>
+      <c r="J27" t="n">
+        <v>175.783634185791</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>7</v>
+      </c>
+      <c r="B28" t="n">
+        <v>27</v>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>sweet</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>sour</t>
+        </is>
+      </c>
+      <c r="E28" t="n">
+        <v>106</v>
+      </c>
+      <c r="F28" t="n">
+        <v>0</v>
+      </c>
+      <c r="G28" t="n">
+        <v>5000</v>
+      </c>
+      <c r="H28" t="n">
+        <v>5000</v>
+      </c>
+      <c r="I28" t="n">
+        <v>5000</v>
+      </c>
+      <c r="J28" t="n">
+        <v>176.506519317627</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>7</v>
+      </c>
+      <c r="B29" t="n">
+        <v>28</v>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>sour</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>sweet</t>
+        </is>
+      </c>
+      <c r="E29" t="n">
+        <v>106</v>
+      </c>
+      <c r="F29" t="n">
+        <v>0</v>
+      </c>
+      <c r="G29" t="n">
+        <v>5000</v>
+      </c>
+      <c r="H29" t="n">
+        <v>5000</v>
+      </c>
+      <c r="I29" t="n">
+        <v>5000</v>
+      </c>
+      <c r="J29" t="n">
+        <v>179.6953678131104</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>8</v>
+      </c>
+      <c r="B30" t="n">
+        <v>29</v>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>sucrose</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>saccarhin</t>
+        </is>
+      </c>
+      <c r="E30" t="n">
+        <v>107</v>
+      </c>
+      <c r="F30" t="n">
+        <v>0</v>
+      </c>
+      <c r="G30" t="n">
+        <v>5000</v>
+      </c>
+      <c r="H30" t="n">
+        <v>5000</v>
+      </c>
+      <c r="I30" t="n">
+        <v>5000</v>
+      </c>
+      <c r="J30" t="n">
+        <v>176.7468452453613</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>8</v>
+      </c>
+      <c r="B31" t="n">
+        <v>30</v>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>sweet</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>sour</t>
+        </is>
+      </c>
+      <c r="E31" t="n">
+        <v>0</v>
+      </c>
+      <c r="F31" t="n">
+        <v>106</v>
+      </c>
+      <c r="G31" t="n">
+        <v>5000</v>
+      </c>
+      <c r="H31" t="n">
+        <v>5000</v>
+      </c>
+      <c r="I31" t="n">
+        <v>5000</v>
+      </c>
+      <c r="J31" t="n">
+        <v>182.2173595428467</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>8</v>
+      </c>
+      <c r="B32" t="n">
+        <v>31</v>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>saccarhin</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>sucrose</t>
+        </is>
+      </c>
+      <c r="E32" t="n">
+        <v>0</v>
+      </c>
+      <c r="F32" t="n">
+        <v>107</v>
+      </c>
+      <c r="G32" t="n">
+        <v>5000</v>
+      </c>
+      <c r="H32" t="n">
+        <v>5000</v>
+      </c>
+      <c r="I32" t="n">
+        <v>5000</v>
+      </c>
+      <c r="J32" t="n">
+        <v>180.6514263153076</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>8</v>
+      </c>
+      <c r="B33" t="n">
+        <v>32</v>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>sour</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>sweet</t>
+        </is>
+      </c>
+      <c r="E33" t="n">
+        <v>0</v>
+      </c>
+      <c r="F33" t="n">
+        <v>106</v>
+      </c>
+      <c r="G33" t="n">
+        <v>5000</v>
+      </c>
+      <c r="H33" t="n">
+        <v>5000</v>
+      </c>
+      <c r="I33" t="n">
+        <v>5000</v>
+      </c>
+      <c r="J33" t="n">
+        <v>180.0343990325928</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>9</v>
+      </c>
+      <c r="B34" t="n">
+        <v>33</v>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>sweet</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>sour</t>
+        </is>
+      </c>
+      <c r="E34" t="n">
+        <v>0</v>
+      </c>
+      <c r="F34" t="n">
+        <v>107</v>
+      </c>
+      <c r="G34" t="n">
+        <v>5000</v>
+      </c>
+      <c r="H34" t="n">
+        <v>5000</v>
+      </c>
+      <c r="I34" t="n">
+        <v>5000</v>
+      </c>
+      <c r="J34" t="n">
+        <v>182.1033954620361</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>9</v>
+      </c>
+      <c r="B35" t="n">
+        <v>34</v>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>saccarhin</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>sucrose</t>
+        </is>
+      </c>
+      <c r="E35" t="n">
+        <v>106</v>
+      </c>
+      <c r="F35" t="n">
+        <v>0</v>
+      </c>
+      <c r="G35" t="n">
+        <v>5000</v>
+      </c>
+      <c r="H35" t="n">
+        <v>5000</v>
+      </c>
+      <c r="I35" t="n">
+        <v>5000</v>
+      </c>
+      <c r="J35" t="n">
+        <v>175.3160953521729</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>9</v>
+      </c>
+      <c r="B36" t="n">
+        <v>35</v>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>sour</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>sweet</t>
+        </is>
+      </c>
+      <c r="E36" t="n">
+        <v>106</v>
+      </c>
+      <c r="F36" t="n">
+        <v>0</v>
+      </c>
+      <c r="G36" t="n">
+        <v>5000</v>
+      </c>
+      <c r="H36" t="n">
+        <v>5000</v>
+      </c>
+      <c r="I36" t="n">
+        <v>5000</v>
+      </c>
+      <c r="J36" t="n">
+        <v>177.9375076293945</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>9</v>
+      </c>
+      <c r="B37" t="n">
+        <v>36</v>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>sucrose</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>saccarhin</t>
+        </is>
+      </c>
+      <c r="E37" t="n">
+        <v>106</v>
+      </c>
+      <c r="F37" t="n">
+        <v>0</v>
+      </c>
+      <c r="G37" t="n">
+        <v>5000</v>
+      </c>
+      <c r="H37" t="n">
+        <v>5000</v>
+      </c>
+      <c r="I37" t="n">
+        <v>5000</v>
+      </c>
+      <c r="J37" t="n">
+        <v>174.7915744781494</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>10</v>
+      </c>
+      <c r="B38" t="n">
+        <v>37</v>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>sucrose</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>saccarhin</t>
+        </is>
+      </c>
+      <c r="E38" t="n">
+        <v>46</v>
+      </c>
+      <c r="F38" t="n">
+        <v>60</v>
+      </c>
+      <c r="G38" t="n">
+        <v>5000</v>
+      </c>
+      <c r="H38" t="n">
+        <v>5000</v>
+      </c>
+      <c r="I38" t="n">
+        <v>5000</v>
+      </c>
+      <c r="J38" t="n">
+        <v>181.55837059021</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>10</v>
+      </c>
+      <c r="B39" t="n">
+        <v>38</v>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>sour</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>sweet</t>
+        </is>
+      </c>
+      <c r="E39" t="n">
+        <v>0</v>
+      </c>
+      <c r="F39" t="n">
+        <v>107</v>
+      </c>
+      <c r="G39" t="n">
+        <v>5000</v>
+      </c>
+      <c r="H39" t="n">
+        <v>5000</v>
+      </c>
+      <c r="I39" t="n">
+        <v>5000</v>
+      </c>
+      <c r="J39" t="n">
+        <v>174.9532222747803</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>10</v>
+      </c>
+      <c r="B40" t="n">
+        <v>39</v>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>saccarhin</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>sucrose</t>
+        </is>
+      </c>
+      <c r="E40" t="n">
+        <v>0</v>
+      </c>
+      <c r="F40" t="n">
+        <v>106</v>
+      </c>
+      <c r="G40" t="n">
+        <v>5000</v>
+      </c>
+      <c r="H40" t="n">
+        <v>5000</v>
+      </c>
+      <c r="I40" t="n">
+        <v>5000</v>
+      </c>
+      <c r="J40" t="n">
+        <v>176.7990589141846</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="n">
+        <v>10</v>
+      </c>
+      <c r="B41" t="n">
+        <v>40</v>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>sweet</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>sour</t>
+        </is>
+      </c>
+      <c r="E41" t="n">
+        <v>0</v>
+      </c>
+      <c r="F41" t="n">
+        <v>106</v>
+      </c>
+      <c r="G41" t="n">
+        <v>5000</v>
+      </c>
+      <c r="H41" t="n">
+        <v>5000</v>
+      </c>
+      <c r="I41" t="n">
+        <v>5000</v>
+      </c>
+      <c r="J41" t="n">
+        <v>178.5287857055664</v>
       </c>
     </row>
   </sheetData>

</xml_diff>